<commit_message>
A LA ONE AGAIN
</commit_message>
<xml_diff>
--- a/client/public/fichiers/ANNEXE 4 - EXEMPLE DE PLAN COMPTABLE ADAPTE.xlsx
+++ b/client/public/fichiers/ANNEXE 4 - EXEMPLE DE PLAN COMPTABLE ADAPTE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://219295cocerto-my.sharepoint.com/personal/lgombaud_cocerto_fr/Documents/SAUVEGARDE LOCAL LG/MEMOIRE DEC/MEMOIRE/ANNEXE/ANNEXE 4 - EXEMPLE DE PLAN COMPTABLE ADAPTE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{EA70746D-6D4A-4C09-95B3-0FC3C3747FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9535C7EB-76B9-4189-A540-296A4796639A}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="8_{EA70746D-6D4A-4C09-95B3-0FC3C3747FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23FC8A03-11C7-4A59-A0FD-F73CF6667E49}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="PCG ADAPTE EDP" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'PCG ADAPTE EDP'!$A$1:$B$195</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'PCG ADAPTE EDP'!$A$1:$B$198</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="246">
   <si>
     <t>NOTICE</t>
   </si>
@@ -1688,6 +1688,15 @@
   </si>
   <si>
     <t>T - Formation continue - Production</t>
+  </si>
+  <si>
+    <t>M - Taxe sur les salaires - Mutualisé</t>
+  </si>
+  <si>
+    <t>NT - Taxe sur les salaires - Pédagogique</t>
+  </si>
+  <si>
+    <t>T - Taxe sur les salaires - Production</t>
   </si>
 </sst>
 </file>
@@ -2508,10 +2517,10 @@
     <tabColor rgb="FF2E8B57"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C325"/>
+  <dimension ref="A1:C328"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3640,495 +3649,510 @@
     </row>
     <row r="141" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>63120</v>
+        <v>63110</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>63121</v>
+        <v>63111</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>63330</v>
+        <v>63112</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>63331</v>
+        <v>63120</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>63332</v>
+        <v>63121</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>63510</v>
+        <v>63330</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>64110</v>
+        <v>63331</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>192</v>
+        <v>241</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>64111</v>
+        <v>63332</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>193</v>
+        <v>242</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>64112</v>
+        <v>63510</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>64120</v>
+        <v>64110</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>64121</v>
+        <v>64111</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>64122</v>
+        <v>64112</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>64510</v>
+        <v>64120</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>64511</v>
+        <v>64121</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>64512</v>
+        <v>64122</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>66110</v>
+        <v>64510</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>67500</v>
+        <v>64511</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>67510</v>
+        <v>64512</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>67520</v>
+        <v>66110</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>67800</v>
+        <v>67500</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>68110</v>
+        <v>67510</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>68111</v>
+        <v>67520</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>68112</v>
+        <v>67800</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>70600</v>
+        <v>68110</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C164" s="14"/>
+        <v>206</v>
+      </c>
     </row>
     <row r="165" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>70601</v>
+        <v>68111</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C165" s="14"/>
+        <v>207</v>
+      </c>
     </row>
     <row r="166" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>70602</v>
+        <v>68112</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C166" s="14"/>
+        <v>208</v>
+      </c>
     </row>
     <row r="167" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>70620</v>
+        <v>70600</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C167" s="14"/>
     </row>
     <row r="168" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>70700</v>
+        <v>70601</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C168" s="14"/>
     </row>
     <row r="169" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>70701</v>
+        <v>70602</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C169" s="14"/>
     </row>
     <row r="170" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>70702</v>
+        <v>70620</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C170" s="14"/>
     </row>
     <row r="171" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>70720</v>
+        <v>70700</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C171" s="14"/>
     </row>
     <row r="172" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>71331</v>
+        <v>70701</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C172" s="14"/>
     </row>
     <row r="173" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>71335</v>
+        <v>70702</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C173" s="14"/>
     </row>
     <row r="174" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>72210</v>
+        <v>70720</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C174" s="14"/>
     </row>
     <row r="175" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>72220</v>
+        <v>71331</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C175" s="14"/>
     </row>
     <row r="176" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>74100</v>
+        <v>71335</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C176" s="14"/>
     </row>
     <row r="177" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>74101</v>
+        <v>72210</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C177" s="14"/>
     </row>
     <row r="178" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>74110</v>
+        <v>72220</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="C178" s="14"/>
     </row>
     <row r="179" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>74111</v>
+        <v>74100</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="C179" s="14"/>
     </row>
     <row r="180" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>74120</v>
+        <v>74101</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C180" s="14"/>
     </row>
     <row r="181" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>74121</v>
+        <v>74110</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C181" s="14"/>
     </row>
     <row r="182" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>74700</v>
+        <v>74111</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="C182" s="14"/>
     </row>
     <row r="183" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>74710</v>
+        <v>74120</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C183" s="14"/>
     </row>
     <row r="184" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>74720</v>
+        <v>74121</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="C184" s="14"/>
     </row>
     <row r="185" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>75410</v>
+        <v>74700</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C185" s="14"/>
     </row>
     <row r="186" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>75420</v>
+        <v>74710</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C186" s="14"/>
     </row>
     <row r="187" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>75610</v>
+        <v>74720</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C187" s="14"/>
     </row>
     <row r="188" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>75620</v>
+        <v>75410</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C188" s="14"/>
     </row>
     <row r="189" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>77500</v>
+        <v>75420</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C189" s="14"/>
     </row>
     <row r="190" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>77510</v>
+        <v>75610</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C190" s="14"/>
     </row>
     <row r="191" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>77520</v>
+        <v>75620</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C191" s="14"/>
     </row>
     <row r="192" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
+        <v>77500</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C192" s="14"/>
+    </row>
+    <row r="193" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
+        <v>77510</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C193" s="14"/>
+    </row>
+    <row r="194" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
+        <v>77520</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C194" s="14"/>
+    </row>
+    <row r="195" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
         <v>77800</v>
       </c>
-      <c r="B192" s="2" t="s">
+      <c r="B195" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C192" s="14"/>
-    </row>
-    <row r="193" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C193" s="14"/>
-    </row>
-    <row r="194" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C194" s="14"/>
-    </row>
-    <row r="195" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C195" s="14"/>
     </row>
-    <row r="196" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C196" s="14"/>
     </row>
-    <row r="197" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C197" s="14"/>
     </row>
-    <row r="198" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C198" s="14"/>
     </row>
-    <row r="199" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C199" s="14"/>
     </row>
-    <row r="200" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C200" s="14"/>
     </row>
-    <row r="201" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C201" s="14"/>
     </row>
-    <row r="202" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C202" s="14"/>
     </row>
-    <row r="203" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C203" s="14"/>
     </row>
-    <row r="204" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C204" s="14"/>
     </row>
-    <row r="205" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C205" s="14"/>
     </row>
-    <row r="206" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C206" s="14"/>
     </row>
-    <row r="207" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C207" s="14"/>
     </row>
-    <row r="208" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C208" s="14"/>
     </row>
     <row r="209" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4215,9 +4239,15 @@
     <row r="236" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C236" s="14"/>
     </row>
-    <row r="237" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C237" s="14"/>
+    </row>
+    <row r="238" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C238" s="14"/>
+    </row>
+    <row r="239" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C239" s="14"/>
+    </row>
     <row r="240" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="241" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="242" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4304,10 +4334,13 @@
     <row r="323" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="324" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="325" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B195">
-    <sortCondition ref="B2:B195"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B198">
+    <sortCondition ref="B2:B198"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>